<commit_message>
progress on DPP dataset
</commit_message>
<xml_diff>
--- a/ISA88-schema-ofetdb.xlsx
+++ b/ISA88-schema-ofetdb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alpha Tauri\Dropbox (GaTech)\Georgia Tech\Virtual Lab Notebook\ofet-db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitHub\ofet-db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9457A97-99B8-401C-8C31-56A27DB55F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB975A1A-45D6-41BA-BD84-B1F26C012144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AB05C28-3B45-46DF-81B3-99556E99ED8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AB05C28-3B45-46DF-81B3-99556E99ED8A}"/>
   </bookViews>
   <sheets>
     <sheet name="OFET PROCESS" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="120">
   <si>
     <t>SAMPLE</t>
   </si>
@@ -140,9 +140,6 @@
     <t>pubchem_CID</t>
   </si>
   <si>
-    <t>IUPAC_name</t>
-  </si>
-  <si>
     <t>STR</t>
   </si>
   <si>
@@ -399,13 +396,16 @@
   </si>
   <si>
     <t>POST_PROCESS_ORDER</t>
+  </si>
+  <si>
+    <t>solvent_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,8 +454,43 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +536,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -870,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1011,6 +1052,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1319,7 +1382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1329,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3318BD9-9F12-4927-8318-E169FD1B0812}">
   <dimension ref="A1:Y73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,15 +1423,17 @@
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="9" t="s">
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="50" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -1391,16 +1456,16 @@
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="52" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -1418,19 +1483,19 @@
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="G3" s="51"/>
+      <c r="H3" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="54" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="38" t="s">
@@ -1447,16 +1512,18 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="G4" s="51"/>
+      <c r="H4" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="55" t="s">
         <v>18</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1473,22 +1540,26 @@
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="G5" s="51"/>
+      <c r="H5" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
       <c r="L5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G6" s="23"/>
-      <c r="H6" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="G6" s="51"/>
+      <c r="H6" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
       <c r="L6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1497,10 +1568,12 @@
       </c>
     </row>
     <row r="7" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G7" s="23"/>
-      <c r="H7" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="G7" s="51"/>
+      <c r="H7" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
       <c r="L7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1509,29 +1582,34 @@
       </c>
     </row>
     <row r="8" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H8" s="24" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="50" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I9" s="4" t="s">
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="52" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I10" s="2" t="s">
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="55" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1586,22 +1664,22 @@
         <v>4</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" s="28" t="s">
         <v>24</v>
@@ -1610,7 +1688,7 @@
         <v>9</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>31</v>
@@ -1619,7 +1697,7 @@
         <v>9</v>
       </c>
       <c r="N19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O19" s="8" t="s">
         <v>30</v>
@@ -1628,7 +1706,7 @@
         <v>9</v>
       </c>
       <c r="Q19" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1639,22 +1717,22 @@
         <v>4</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>25</v>
@@ -1677,28 +1755,28 @@
     </row>
     <row r="21" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>27</v>
@@ -1721,37 +1799,37 @@
     </row>
     <row r="22" spans="1:25" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M22" s="13" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>29</v>
@@ -1765,28 +1843,28 @@
         <v>4</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O23" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -1797,31 +1875,31 @@
         <v>4</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>9</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>9</v>
@@ -1829,19 +1907,19 @@
     </row>
     <row r="25" spans="1:25" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D25" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L25" s="10" t="s">
         <v>28</v>
@@ -1858,19 +1936,19 @@
     </row>
     <row r="26" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D26" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L26" s="19" t="s">
         <v>32</v>
@@ -1879,36 +1957,36 @@
         <v>4</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D27" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L27" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="M27" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="M27" s="17" t="s">
-        <v>34</v>
-      </c>
       <c r="O27" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P27" s="22" t="s">
         <v>29</v>
@@ -1916,28 +1994,28 @@
     </row>
     <row r="28" spans="1:25" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D28" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M28" s="17" t="s">
         <v>29</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P28" s="22" t="s">
         <v>29</v>
@@ -1945,19 +2023,19 @@
     </row>
     <row r="29" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D29" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>7</v>
@@ -1966,30 +2044,30 @@
         <v>18</v>
       </c>
       <c r="O29" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P29" s="22" t="s">
         <v>29</v>
       </c>
       <c r="Q29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D30" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
@@ -2002,74 +2080,74 @@
     </row>
     <row r="31" spans="1:25" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D31" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D32" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D33" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I33" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K33" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M33" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N33" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P33" s="9" t="s">
         <v>9</v>
@@ -2077,16 +2155,16 @@
     </row>
     <row r="34" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D34" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I34" s="44" t="s">
         <v>20</v>
@@ -2101,7 +2179,7 @@
         <v>2</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P34" s="11" t="s">
         <v>2</v>
@@ -2109,58 +2187,58 @@
     </row>
     <row r="35" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D35" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="L35" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M35" s="31" t="s">
         <v>4</v>
       </c>
       <c r="O35" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P35" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D36" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="L36" s="46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M36" s="47" t="s">
         <v>4</v>
       </c>
       <c r="O36" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P36" s="42" t="s">
         <v>18</v>
@@ -2168,16 +2246,16 @@
     </row>
     <row r="37" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D37" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F37" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
@@ -2190,54 +2268,54 @@
     </row>
     <row r="38" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D38" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
     <row r="39" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D39" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="18"/>
     </row>
     <row r="40" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D40" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F40" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G40" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H40" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>9</v>
@@ -2245,18 +2323,18 @@
     </row>
     <row r="41" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D41" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G41" s="29"/>
       <c r="H41" s="18"/>
       <c r="I41" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>2</v>
@@ -2264,17 +2342,17 @@
     </row>
     <row r="42" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D42" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G42" s="29"/>
       <c r="I42" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J42" s="37" t="s">
         <v>18</v>
@@ -2282,168 +2360,168 @@
     </row>
     <row r="43" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D43" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F43" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J43" s="37"/>
     </row>
     <row r="44" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D44" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I44" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J44" s="37"/>
     </row>
     <row r="45" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D45" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F45" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I45" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J45" s="37"/>
     </row>
     <row r="46" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D46" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F46" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I46" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J46" s="37"/>
       <c r="O46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D47" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F47" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J47" s="17"/>
     </row>
     <row r="48" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D48" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F48" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J48" s="17"/>
     </row>
     <row r="49" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D49" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I49" s="12"/>
       <c r="J49" s="13"/>
     </row>
     <row r="50" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D50" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D51" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F51" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D52" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F52" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G52" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H52" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K52" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N52" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P52" s="9" t="s">
         <v>9</v>
@@ -2451,25 +2529,25 @@
     </row>
     <row r="53" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D53" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J53" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M53" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O53" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P53" s="11" t="s">
         <v>2</v>
@@ -2477,39 +2555,39 @@
     </row>
     <row r="54" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D54" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L54" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M54" s="31" t="s">
         <v>4</v>
       </c>
       <c r="O54" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P54" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D55" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L55" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M55" s="33" t="s">
         <v>4</v>
       </c>
       <c r="O55" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P55" s="42" t="s">
         <v>18</v>
@@ -2517,10 +2595,10 @@
     </row>
     <row r="56" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D56" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O56" s="39" t="s">
         <v>7</v>
@@ -2531,57 +2609,57 @@
     </row>
     <row r="57" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D57" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D58" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D59" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D60" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H60" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J60" s="9" t="s">
         <v>9</v>
       </c>
       <c r="L60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D61" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I61" s="10" t="s">
         <v>21</v>
@@ -2590,29 +2668,29 @@
         <v>2</v>
       </c>
       <c r="L61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D62" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J62" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D63" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I63" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J63" s="17" t="s">
         <v>18</v>
@@ -2620,7 +2698,7 @@
     </row>
     <row r="64" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D64" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I64" s="34" t="s">
         <v>7</v>
@@ -2631,60 +2709,60 @@
     </row>
     <row r="65" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D65" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D66" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D67" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D68" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D69" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G69" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H69" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J69" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K69" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M69" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N69" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O69" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P69" s="9" t="s">
         <v>9</v>
@@ -2692,19 +2770,19 @@
     </row>
     <row r="70" spans="4:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I70" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J70" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L70" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M70" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O70" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P70" s="11" t="s">
         <v>2</v>
@@ -2712,27 +2790,27 @@
     </row>
     <row r="71" spans="4:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L71" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M71" s="31" t="s">
         <v>4</v>
       </c>
       <c r="O71" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P71" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="4:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L72" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M72" s="33" t="s">
         <v>4</v>
       </c>
       <c r="O72" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P72" s="42" t="s">
         <v>18</v>
@@ -2740,10 +2818,10 @@
     </row>
     <row r="73" spans="4:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L73" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M73" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O73" s="39" t="s">
         <v>7</v>
@@ -2826,13 +2904,13 @@
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>9</v>
@@ -2846,10 +2924,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>3</v>
@@ -2860,20 +2938,20 @@
     </row>
     <row r="12" spans="1:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -2881,7 +2959,7 @@
       <c r="B13" s="2"/>
       <c r="C13" s="23"/>
       <c r="D13" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>7</v>
@@ -2893,27 +2971,27 @@
     <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C14" s="23"/>
       <c r="D14" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C15" s="23"/>
       <c r="D15" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C16" s="23"/>
       <c r="D16" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="4:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D17" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>9</v>
@@ -3060,127 +3138,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed DPP dataset formatting
</commit_message>
<xml_diff>
--- a/ISA88-schema-ofetdb.xlsx
+++ b/ISA88-schema-ofetdb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliu319\Documents\GitHub\ofet-db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitHub\ofet-db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943D8BA3-8E5E-453C-A1EA-7A2D975247FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6B23C2-06CF-4E22-921E-C72F67C07BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9AB05C28-3B45-46DF-81B3-99556E99ED8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AB05C28-3B45-46DF-81B3-99556E99ED8A}"/>
   </bookViews>
   <sheets>
     <sheet name="OFET PROCESS" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="119">
   <si>
     <t>SAMPLE</t>
   </si>
@@ -98,9 +98,6 @@
     <t>JSONB</t>
   </si>
   <si>
-    <t>solution_makeup_id</t>
-  </si>
-  <si>
     <t>solution_treatment_id</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
   </si>
   <si>
     <t>OFET_PROCESS</t>
-  </si>
-  <si>
-    <t>post_processing_id</t>
   </si>
   <si>
     <t>SOLUTION</t>
@@ -1327,7 +1321,7 @@
   <dimension ref="A1:Y73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1330,7 @@
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="40.5703125" customWidth="1"/>
     <col min="10" max="10" width="35.28515625" customWidth="1"/>
     <col min="12" max="12" width="51" bestFit="1" customWidth="1"/>
@@ -1357,7 +1351,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
@@ -1397,10 +1391,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I3" s="36" t="s">
         <v>1</v>
@@ -1435,7 +1429,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>11</v>
@@ -1460,7 +1454,7 @@
     <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:25" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
@@ -1502,96 +1496,96 @@
     </row>
     <row r="19" spans="1:25" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M20" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>2</v>
@@ -1599,43 +1593,43 @@
     </row>
     <row r="21" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M21" s="15" t="s">
         <v>4</v>
       </c>
       <c r="O21" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P21" s="15" t="s">
         <v>4</v>
@@ -1643,107 +1637,107 @@
     </row>
     <row r="22" spans="1:25" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O23" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>9</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>9</v>
@@ -1751,28 +1745,28 @@
     </row>
     <row r="25" spans="1:25" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D25" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M25" s="11" t="s">
         <v>4</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P25" s="11" t="s">
         <v>2</v>
@@ -1780,126 +1774,126 @@
     </row>
     <row r="26" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D26" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O26" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="M26" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="O26" s="23" t="s">
-        <v>42</v>
-      </c>
       <c r="P26" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D27" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L27" s="32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M27" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D28" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O28" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P28" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D29" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D30" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
@@ -1912,74 +1906,74 @@
     </row>
     <row r="31" spans="1:25" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D31" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D32" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H32" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D33" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I33" s="26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M33" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N33" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P33" s="9" t="s">
         <v>9</v>
@@ -1987,31 +1981,31 @@
     </row>
     <row r="34" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D34" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I34" s="42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J34" s="43" t="s">
         <v>2</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M34" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P34" s="11" t="s">
         <v>2</v>
@@ -2019,58 +2013,58 @@
     </row>
     <row r="35" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D35" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="L35" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M35" s="29" t="s">
         <v>4</v>
       </c>
       <c r="O35" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P35" s="40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D36" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="L36" s="44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M36" s="45" t="s">
         <v>4</v>
       </c>
       <c r="O36" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P36" s="40" t="s">
         <v>18</v>
@@ -2078,16 +2072,16 @@
     </row>
     <row r="37" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D37" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
@@ -2100,54 +2094,54 @@
     </row>
     <row r="38" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D38" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
     <row r="39" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D39" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="18"/>
     </row>
     <row r="40" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D40" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>9</v>
@@ -2155,18 +2149,18 @@
     </row>
     <row r="41" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D41" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="18"/>
       <c r="I41" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>2</v>
@@ -2174,17 +2168,17 @@
     </row>
     <row r="42" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D42" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G42" s="27"/>
       <c r="I42" s="34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J42" s="35" t="s">
         <v>18</v>
@@ -2192,168 +2186,168 @@
     </row>
     <row r="43" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D43" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I43" s="34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J43" s="35"/>
     </row>
     <row r="44" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D44" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I44" s="34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J44" s="35"/>
     </row>
     <row r="45" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D45" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F45" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I45" s="34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J45" s="35"/>
     </row>
     <row r="46" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D46" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I46" s="34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J46" s="35"/>
       <c r="O46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D47" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F47" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J47" s="17"/>
     </row>
     <row r="48" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D48" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F48" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J48" s="17"/>
     </row>
     <row r="49" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D49" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F49" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I49" s="12"/>
       <c r="J49" s="13"/>
     </row>
     <row r="50" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D50" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F50" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D51" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F51" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D52" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F52" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N52" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P52" s="9" t="s">
         <v>9</v>
@@ -2361,25 +2355,25 @@
     </row>
     <row r="53" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D53" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J53" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M53" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O53" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P53" s="11" t="s">
         <v>2</v>
@@ -2387,39 +2381,39 @@
     </row>
     <row r="54" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D54" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L54" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M54" s="29" t="s">
         <v>4</v>
       </c>
       <c r="O54" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P54" s="40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D55" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L55" s="30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M55" s="31" t="s">
         <v>4</v>
       </c>
       <c r="O55" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P55" s="40" t="s">
         <v>18</v>
@@ -2427,10 +2421,10 @@
     </row>
     <row r="56" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D56" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O56" s="37" t="s">
         <v>7</v>
@@ -2441,88 +2435,88 @@
     </row>
     <row r="57" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D57" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D58" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D59" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E59" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D60" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G60" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H60" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J60" s="9" t="s">
         <v>9</v>
       </c>
       <c r="L60" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D61" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J61" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D62" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J62" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D63" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I63" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J63" s="17" t="s">
         <v>18</v>
@@ -2530,7 +2524,7 @@
     </row>
     <row r="64" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D64" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I64" s="32" t="s">
         <v>7</v>
@@ -2541,60 +2535,60 @@
     </row>
     <row r="65" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D65" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D66" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="4:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D67" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D68" s="27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D69" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G69" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H69" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J69" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K69" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M69" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N69" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O69" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P69" s="9" t="s">
         <v>9</v>
@@ -2602,19 +2596,19 @@
     </row>
     <row r="70" spans="4:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I70" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J70" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L70" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M70" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O70" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P70" s="11" t="s">
         <v>2</v>
@@ -2622,27 +2616,27 @@
     </row>
     <row r="71" spans="4:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L71" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M71" s="29" t="s">
         <v>4</v>
       </c>
       <c r="O71" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P71" s="40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="4:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L72" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M72" s="31" t="s">
         <v>4</v>
       </c>
       <c r="O72" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P72" s="40" t="s">
         <v>18</v>
@@ -2650,10 +2644,10 @@
     </row>
     <row r="73" spans="4:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L73" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M73" s="33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O73" s="37" t="s">
         <v>7</v>
@@ -2736,13 +2730,13 @@
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>9</v>
@@ -2756,10 +2750,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>3</v>
@@ -2770,20 +2764,20 @@
     </row>
     <row r="12" spans="1:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -2791,7 +2785,7 @@
       <c r="B13" s="2"/>
       <c r="C13" s="21"/>
       <c r="D13" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>7</v>
@@ -2803,27 +2797,27 @@
     <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C14" s="21"/>
       <c r="D14" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C15" s="21"/>
       <c r="D15" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C16" s="21"/>
       <c r="D16" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D17" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>9</v>
@@ -2970,127 +2964,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished DPPDTT dataset upload to local db
</commit_message>
<xml_diff>
--- a/ISA88-schema-ofetdb.xlsx
+++ b/ISA88-schema-ofetdb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliu319\Documents\GitHub\ofet-db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitHub\ofet-db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFD1A44-4B1F-40BC-AAB1-78BAF9A929C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C238A56-81E6-49B8-B9BF-058EFAB56245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9AB05C28-3B45-46DF-81B3-99556E99ED8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AB05C28-3B45-46DF-81B3-99556E99ED8A}"/>
   </bookViews>
   <sheets>
     <sheet name="OFET PROCESS" sheetId="1" r:id="rId1"/>
@@ -209,18 +209,12 @@
     <t>post_process_step_id</t>
   </si>
   <si>
-    <t>post_process_type</t>
-  </si>
-  <si>
     <t>POST_PROCESS_STEP</t>
   </si>
   <si>
     <t>deposition_type</t>
   </si>
   <si>
-    <t>deposition_parameters</t>
-  </si>
-  <si>
     <t>JSON TYPES</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     <t>filename</t>
   </si>
   <si>
-    <t>parameters</t>
-  </si>
-  <si>
     <t>SAMPLE.meta</t>
   </si>
   <si>
@@ -396,6 +387,15 @@
   </si>
   <si>
     <t>dielectric_thickness</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>measurement_type</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -972,9 +972,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1317,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3318BD9-9F12-4927-8318-E169FD1B0812}">
   <dimension ref="A1:Y73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1345,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
@@ -1388,10 +1385,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" s="35" t="s">
         <v>1</v>
@@ -1408,11 +1405,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="F4" s="2"/>
       <c r="I4" s="5" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>11</v>
@@ -1420,13 +1417,13 @@
     </row>
     <row r="5" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>11</v>
@@ -1442,7 +1439,7 @@
     </row>
     <row r="7" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I7" s="2" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>17</v>
@@ -1614,7 +1611,7 @@
         <v>35</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J21" s="13" t="s">
         <v>26</v>
@@ -1658,13 +1655,13 @@
         <v>35</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M22" s="13" t="s">
         <v>26</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>26</v>
@@ -1757,7 +1754,7 @@
         <v>35</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M25" s="11" t="s">
         <v>4</v>
@@ -1786,13 +1783,13 @@
         <v>35</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M26" s="17" t="s">
         <v>29</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P26" s="23" t="s">
         <v>29</v>
@@ -1815,13 +1812,13 @@
         <v>35</v>
       </c>
       <c r="L27" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M27" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P27" s="20" t="s">
         <v>29</v>
@@ -1844,7 +1841,7 @@
         <v>35</v>
       </c>
       <c r="O28" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="P28" s="20" t="s">
         <v>26</v>
@@ -1867,7 +1864,7 @@
         <v>35</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P29" s="20" t="s">
         <v>26</v>
@@ -1918,7 +1915,7 @@
         <v>35</v>
       </c>
       <c r="O31" s="12" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="P31" s="13" t="s">
         <v>18</v>
@@ -1967,7 +1964,7 @@
         <v>34</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M33" s="9" t="s">
         <v>9</v>
@@ -1995,10 +1992,10 @@
       <c r="G34" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="42" t="s">
+      <c r="J34" s="41" t="s">
         <v>2</v>
       </c>
       <c r="L34" s="10" t="s">
@@ -2035,10 +2032,10 @@
       <c r="M35" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O35" s="38" t="s">
+      <c r="O35" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P35" s="39" t="s">
+      <c r="P35" s="38" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2060,16 +2057,16 @@
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
-      <c r="L36" s="43" t="s">
+      <c r="L36" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="M36" s="44" t="s">
+      <c r="M36" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="O36" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="P36" s="39" t="s">
+      <c r="O36" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="P36" s="38" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2088,10 +2085,10 @@
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
-      <c r="O37" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="P37" s="37" t="s">
+      <c r="O37" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="P37" s="36" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2181,7 +2178,7 @@
       </c>
       <c r="G42" s="26"/>
       <c r="I42" s="33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J42" s="34" t="s">
         <v>18</v>
@@ -2198,7 +2195,7 @@
         <v>35</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J43" s="34"/>
     </row>
@@ -2213,7 +2210,7 @@
         <v>35</v>
       </c>
       <c r="I44" s="33" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J44" s="34"/>
     </row>
@@ -2243,7 +2240,7 @@
         <v>35</v>
       </c>
       <c r="I46" s="33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J46" s="34"/>
       <c r="O46" t="s">
@@ -2261,7 +2258,7 @@
         <v>35</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J47" s="17"/>
     </row>
@@ -2276,7 +2273,7 @@
         <v>35</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J48" s="17"/>
     </row>
@@ -2291,7 +2288,7 @@
         <v>35</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="J49" s="13" t="s">
         <v>18</v>
@@ -2345,7 +2342,7 @@
         <v>34</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M52" s="9" t="s">
         <v>9</v>
@@ -2380,7 +2377,7 @@
         <v>2</v>
       </c>
       <c r="O53" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P53" s="11" t="s">
         <v>2</v>
@@ -2399,10 +2396,10 @@
       <c r="M54" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O54" s="38" t="s">
+      <c r="O54" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P54" s="39" t="s">
+      <c r="P54" s="38" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2414,15 +2411,15 @@
         <v>35</v>
       </c>
       <c r="L55" s="29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M55" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="O55" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="P55" s="39" t="s">
+      <c r="O55" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="P55" s="38" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2433,10 +2430,10 @@
       <c r="E56" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="O56" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="P56" s="37" t="s">
+      <c r="O56" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="P56" s="36" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2487,7 +2484,7 @@
         <v>9</v>
       </c>
       <c r="L60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="4:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -2501,7 +2498,7 @@
         <v>2</v>
       </c>
       <c r="L61" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -2509,13 +2506,13 @@
         <v>35</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J62" s="17" t="s">
         <v>29</v>
       </c>
       <c r="L62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="4:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -2523,7 +2520,7 @@
         <v>35</v>
       </c>
       <c r="I63" s="16" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="J63" s="17" t="s">
         <v>18</v>
@@ -2534,7 +2531,7 @@
         <v>35</v>
       </c>
       <c r="I64" s="31" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="J64" s="32" t="s">
         <v>18</v>
@@ -2586,7 +2583,7 @@
         <v>34</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M69" s="9" t="s">
         <v>9</v>
@@ -2595,7 +2592,7 @@
         <v>34</v>
       </c>
       <c r="O69" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P69" s="9" t="s">
         <v>9</v>
@@ -2628,10 +2625,10 @@
       <c r="M71" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O71" s="38" t="s">
+      <c r="O71" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P71" s="39" t="s">
+      <c r="P71" s="38" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2642,24 +2639,24 @@
       <c r="M72" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="O72" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="P72" s="39" t="s">
+      <c r="O72" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="P72" s="38" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="73" spans="4:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L73" s="31" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="M73" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="O73" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="P73" s="37" t="s">
+      <c r="O73" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="P73" s="36" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2737,13 +2734,13 @@
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>9</v>
@@ -2757,7 +2754,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>34</v>
@@ -2771,20 +2768,20 @@
     </row>
     <row r="12" spans="1:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="22" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -2821,10 +2818,10 @@
     </row>
     <row r="17" spans="4:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D17" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>9</v>
@@ -2971,127 +2968,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>